<commit_message>
changed into a snakemake workflow
</commit_message>
<xml_diff>
--- a/output/DEG/Filter_DEG_Run29_D8_WT_KO.xlsx
+++ b/output/DEG/Filter_DEG_Run29_D8_WT_KO.xlsx
@@ -779,19 +779,19 @@
         <v>356.958232528948</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.47470383180943</v>
+        <v>-1.47470357171424</v>
       </c>
       <c r="C2" t="n">
-        <v>0.216645102153119</v>
+        <v>0.216639014157499</v>
       </c>
       <c r="D2" t="n">
-        <v>-6.80700286853082</v>
+        <v>-6.80719295852275</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00000000000996529452935981</v>
+        <v>0.00000000000995214111789237</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00000000217352629447215</v>
+        <v>0.0000000021706574093025</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -802,19 +802,19 @@
         <v>81.6202450681396</v>
       </c>
       <c r="B3" t="n">
-        <v>2.41022069105794</v>
+        <v>2.41022082334188</v>
       </c>
       <c r="C3" t="n">
-        <v>0.315484623531111</v>
+        <v>0.315478844346186</v>
       </c>
       <c r="D3" t="n">
-        <v>7.63974061265226</v>
+        <v>7.63988098262797</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0000000000000217659788490665</v>
+        <v>0.0000000000000217422626832164</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00000000000693115830469673</v>
+        <v>0.00000000000692360612884342</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -825,19 +825,19 @@
         <v>117.412564401226</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.38610328615736</v>
+        <v>-1.38610327739066</v>
       </c>
       <c r="C4" t="n">
-        <v>0.19470421517346</v>
+        <v>0.194706585093929</v>
       </c>
       <c r="D4" t="n">
-        <v>-7.11902043272404</v>
+        <v>-7.11893373674024</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00000000000108696797221056</v>
+        <v>0.00000000000108765180947521</v>
       </c>
       <c r="F4" t="n">
-        <v>0.000000000266256985439024</v>
+        <v>0.000000000266424494007143</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -848,19 +848,19 @@
         <v>60.6394340641106</v>
       </c>
       <c r="B5" t="n">
-        <v>1.6601594607625</v>
+        <v>1.66015950097778</v>
       </c>
       <c r="C5" t="n">
-        <v>0.312326034430769</v>
+        <v>0.312322738997531</v>
       </c>
       <c r="D5" t="n">
-        <v>5.31546934211946</v>
+        <v>5.31552555637297</v>
       </c>
       <c r="E5" t="n">
-        <v>0.000000106382760910345</v>
+        <v>0.00000010634992137983</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0000106529957183303</v>
+        <v>0.0000106497072214443</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -871,19 +871,19 @@
         <v>99.9660821798489</v>
       </c>
       <c r="B6" t="n">
-        <v>1.12738455891202</v>
+        <v>1.12738444942314</v>
       </c>
       <c r="C6" t="n">
-        <v>0.287452074043646</v>
+        <v>0.287445598293987</v>
       </c>
       <c r="D6" t="n">
-        <v>3.92199138817428</v>
+        <v>3.92207936428408</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0000878201317542939</v>
+        <v>0.0000877880640802753</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00365084109084038</v>
+        <v>0.00364950797985938</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -894,19 +894,19 @@
         <v>139.489555467103</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.67684393260987</v>
+        <v>-2.67684359833987</v>
       </c>
       <c r="C7" t="n">
-        <v>0.245215906985138</v>
+        <v>0.245212204883819</v>
       </c>
       <c r="D7" t="n">
-        <v>-10.9162736036211</v>
+        <v>-10.9164370493228</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000000000000000000000000000963689861727379</v>
+        <v>0.00000000000000000000000000096195777819242</v>
       </c>
       <c r="F7" t="n">
-        <v>0.000000000000000000000000767193498921167</v>
+        <v>0.000000000000000000000000765814587218985</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -917,19 +917,19 @@
         <v>135.457306545442</v>
       </c>
       <c r="B8" t="n">
-        <v>1.2428129088145</v>
+        <v>1.24281286396878</v>
       </c>
       <c r="C8" t="n">
-        <v>0.338319262807603</v>
+        <v>0.338305992038501</v>
       </c>
       <c r="D8" t="n">
-        <v>3.67349141902472</v>
+        <v>3.67363538694681</v>
       </c>
       <c r="E8" t="n">
-        <v>0.000239258715604841</v>
+        <v>0.00023912388483832</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00836111348232339</v>
+        <v>0.00836152896210043</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
@@ -940,19 +940,19 @@
         <v>189.905793916155</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.37358124717695</v>
+        <v>-1.3735812811793</v>
       </c>
       <c r="C9" t="n">
-        <v>0.176514672142376</v>
+        <v>0.176515160233944</v>
       </c>
       <c r="D9" t="n">
-        <v>-7.78168313435738</v>
+        <v>-7.78166180943795</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00000000000000715659359821989</v>
+        <v>0.00000000000000715780030242944</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00000000000258971098342857</v>
+        <v>0.00000000000259014764580185</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -963,19 +963,19 @@
         <v>175.455757809847</v>
       </c>
       <c r="B10" t="n">
-        <v>1.10225145424974</v>
+        <v>1.10225160218633</v>
       </c>
       <c r="C10" t="n">
-        <v>0.214018249655989</v>
+        <v>0.214015016558267</v>
       </c>
       <c r="D10" t="n">
-        <v>5.15026852159332</v>
+        <v>5.15034701729087</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000000260113783158377</v>
+        <v>0.00000026000493781932</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0000231370483544563</v>
+        <v>0.0000231273665919509</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
@@ -986,19 +986,19 @@
         <v>69.9418513277101</v>
       </c>
       <c r="B11" t="n">
-        <v>2.08297291989604</v>
+        <v>2.0829731840557</v>
       </c>
       <c r="C11" t="n">
-        <v>0.381298014204905</v>
+        <v>0.381286727754586</v>
       </c>
       <c r="D11" t="n">
-        <v>5.4628475425961</v>
+        <v>5.46300994089781</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0000000468556990215291</v>
+        <v>0.0000000468128374357451</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00000514507889531577</v>
+        <v>0.00000514037239759954</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -1009,19 +1009,19 @@
         <v>310.125173485474</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.60499288784394</v>
+        <v>-2.60499302760844</v>
       </c>
       <c r="C12" t="n">
-        <v>0.195017207996799</v>
+        <v>0.195013816580646</v>
       </c>
       <c r="D12" t="n">
-        <v>-13.3577591157325</v>
+        <v>-13.3579921324763</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000000000000000000000000000000000000000106728990454777</v>
+        <v>0.00000000000000000000000000000000000000010639546559866</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000000000000000000000000000000000000188815442891218</v>
+        <v>0.000000000000000000000000000000000000188225400362429</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
@@ -1032,19 +1032,19 @@
         <v>3573.57061663105</v>
       </c>
       <c r="B13" t="n">
-        <v>1.34925573995193</v>
+        <v>1.34925574961975</v>
       </c>
       <c r="C13" t="n">
-        <v>0.123825986852047</v>
+        <v>0.12382462622984</v>
       </c>
       <c r="D13" t="n">
-        <v>10.8963859223192</v>
+        <v>10.8965057331593</v>
       </c>
       <c r="E13" t="n">
-        <v>0.00000000000000000000000000119926624549445</v>
+        <v>0.00000000000000000000000000119768865405724</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0000000000000000000000009092722457506</v>
+        <v>0.000000000000000000000000908076130947591</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -1055,19 +1055,19 @@
         <v>133.435161072282</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.06200812593559</v>
+        <v>-1.06200814357911</v>
       </c>
       <c r="C14" t="n">
-        <v>0.198419131075629</v>
+        <v>0.198419604920233</v>
       </c>
       <c r="D14" t="n">
-        <v>-5.352347428287</v>
+        <v>-5.35233473530024</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0000000868204987146039</v>
+        <v>0.0000000868265908051305</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00000897633753593456</v>
+        <v>0.00000897696739480057</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
@@ -1078,19 +1078,19 @@
         <v>61.1127048739596</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.51697436622303</v>
+        <v>-1.51697413075575</v>
       </c>
       <c r="C15" t="n">
-        <v>0.367364355762113</v>
+        <v>0.367354105739669</v>
       </c>
       <c r="D15" t="n">
-        <v>-4.12934554599345</v>
+        <v>-4.1294601232272</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0000363797298426063</v>
+        <v>0.0000363616059848924</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00172392279331541</v>
+        <v>0.001723063959796</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
@@ -1101,19 +1101,19 @@
         <v>187.340746486496</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.71051943360114</v>
+        <v>-1.71051955385096</v>
       </c>
       <c r="C16" t="n">
-        <v>0.231628652550704</v>
+        <v>0.231623413793384</v>
       </c>
       <c r="D16" t="n">
-        <v>-7.38474888475511</v>
+        <v>-7.38491642894445</v>
       </c>
       <c r="E16" t="n">
-        <v>0.000000000000152741387477408</v>
+        <v>0.000000000000152549175218891</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0000000000434276494895588</v>
+        <v>0.0000000000433729994256284</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
@@ -1124,19 +1124,19 @@
         <v>413.337075278206</v>
       </c>
       <c r="B17" t="n">
-        <v>3.02564532362602</v>
+        <v>3.02564547919425</v>
       </c>
       <c r="C17" t="n">
-        <v>0.241947430571283</v>
+        <v>0.241938883949042</v>
       </c>
       <c r="D17" t="n">
-        <v>12.5053831589858</v>
+        <v>12.505825561432</v>
       </c>
       <c r="E17" t="n">
-        <v>0.00000000000000000000000000000000000697626352278087</v>
+        <v>0.00000000000000000000000000000000000693753145988054</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00000000000000000000000000000000925633898414309</v>
+        <v>0.00000000000000000000000000000000920494799201816</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
@@ -1147,19 +1147,19 @@
         <v>202.083553073347</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.47568906697129</v>
+        <v>-1.47568914071407</v>
       </c>
       <c r="C18" t="n">
-        <v>0.253124493777771</v>
+        <v>0.253116915086706</v>
       </c>
       <c r="D18" t="n">
-        <v>-5.8298943928629</v>
+        <v>-5.83006923977629</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00000000554624648966698</v>
+        <v>0.0000000055404382004741</v>
       </c>
       <c r="F18" t="n">
-        <v>0.000000754763560756219</v>
+        <v>0.000000753973136991014</v>
       </c>
       <c r="G18" t="s">
         <v>23</v>
@@ -1170,19 +1170,19 @@
         <v>191.775869634096</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.54726449230046</v>
+        <v>-1.54726463935762</v>
       </c>
       <c r="C19" t="n">
-        <v>0.312586807290148</v>
+        <v>0.312573407194506</v>
       </c>
       <c r="D19" t="n">
-        <v>-4.94987138361302</v>
+        <v>-4.95008405623835</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00000074262541231727</v>
+        <v>0.000000741814359199321</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0000579611853672332</v>
+        <v>0.0000578978834665274</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>
@@ -1193,19 +1193,19 @@
         <v>612.531247162727</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.02732235824488</v>
+        <v>-1.02732234867187</v>
       </c>
       <c r="C20" t="n">
-        <v>0.126263008232071</v>
+        <v>0.126263472056687</v>
       </c>
       <c r="D20" t="n">
-        <v>-8.13636846317387</v>
+        <v>-8.13633849868035</v>
       </c>
       <c r="E20" t="n">
-        <v>0.000000000000000407310928983123</v>
+        <v>0.000000000000000407411702359029</v>
       </c>
       <c r="F20" t="n">
-        <v>0.000000000000170663279243929</v>
+        <v>0.000000000000170705503288433</v>
       </c>
       <c r="G20" t="s">
         <v>25</v>
@@ -1216,19 +1216,19 @@
         <v>155.010283558484</v>
       </c>
       <c r="B21" t="n">
-        <v>-1.4081743559539</v>
+        <v>-1.40817512754304</v>
       </c>
       <c r="C21" t="n">
-        <v>0.282762163566325</v>
+        <v>0.282753029807844</v>
       </c>
       <c r="D21" t="n">
-        <v>-4.98006642116952</v>
+        <v>-4.9802300208773</v>
       </c>
       <c r="E21" t="n">
-        <v>0.000000635624541628435</v>
+        <v>0.000000635087431197153</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0000506020697590397</v>
+        <v>0.0000505593103976053</v>
       </c>
       <c r="G21" t="s">
         <v>26</v>
@@ -1239,19 +1239,19 @@
         <v>1314.523155922</v>
       </c>
       <c r="B22" t="n">
-        <v>1.14980094438434</v>
+        <v>1.14980094932404</v>
       </c>
       <c r="C22" t="n">
-        <v>0.188593571936477</v>
+        <v>0.188587441853397</v>
       </c>
       <c r="D22" t="n">
-        <v>6.09671333215757</v>
+        <v>6.09691153357849</v>
       </c>
       <c r="E22" t="n">
-        <v>0.00000000108271427448179</v>
+        <v>0.000000001081373238904</v>
       </c>
       <c r="F22" t="n">
-        <v>0.000000174131077558576</v>
+        <v>0.000000173915401109389</v>
       </c>
       <c r="G22" t="s">
         <v>27</v>
@@ -1262,19 +1262,19 @@
         <v>73.2343404512584</v>
       </c>
       <c r="B23" t="n">
-        <v>1.83288452483393</v>
+        <v>1.83288457494228</v>
       </c>
       <c r="C23" t="n">
-        <v>0.376478661766336</v>
+        <v>0.376467124802852</v>
       </c>
       <c r="D23" t="n">
-        <v>4.86849511266994</v>
+        <v>4.86864444246526</v>
       </c>
       <c r="E23" t="n">
-        <v>0.00000112451303351673</v>
+        <v>0.00000112366375206733</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0000832767279983876</v>
+        <v>0.0000832138337693771</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -1285,19 +1285,19 @@
         <v>229.432528253506</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.49083245425179</v>
+        <v>-1.49083225399906</v>
       </c>
       <c r="C24" t="n">
-        <v>0.186431854649511</v>
+        <v>0.186429747659077</v>
       </c>
       <c r="D24" t="n">
-        <v>-7.99666160621815</v>
+        <v>-7.99675090868727</v>
       </c>
       <c r="E24" t="n">
-        <v>0.00000000000000127837948406985</v>
+        <v>0.00000000000000127745303533099</v>
       </c>
       <c r="F24" t="n">
-        <v>0.000000000000508858953634004</v>
+        <v>0.000000000000508490180713499</v>
       </c>
       <c r="G24" t="s">
         <v>29</v>
@@ -1308,19 +1308,19 @@
         <v>201.160848596615</v>
       </c>
       <c r="B25" t="n">
-        <v>-1.5592109427593</v>
+        <v>-1.55921063545422</v>
       </c>
       <c r="C25" t="n">
-        <v>0.233573954902218</v>
+        <v>0.233568030484451</v>
       </c>
       <c r="D25" t="n">
-        <v>-6.67544865356258</v>
+        <v>-6.67561665960965</v>
       </c>
       <c r="E25" t="n">
-        <v>0.0000000000246476951324168</v>
+        <v>0.0000000000246194730034821</v>
       </c>
       <c r="F25" t="n">
-        <v>0.00000000496760255567519</v>
+        <v>0.00000000496191454634737</v>
       </c>
       <c r="G25" t="s">
         <v>30</v>
@@ -1331,19 +1331,19 @@
         <v>423.985953690047</v>
       </c>
       <c r="B26" t="n">
-        <v>-1.04240162400304</v>
+        <v>-1.04240145932088</v>
       </c>
       <c r="C26" t="n">
-        <v>0.107652693529559</v>
+        <v>0.107656669347705</v>
       </c>
       <c r="D26" t="n">
-        <v>-9.68300550433347</v>
+        <v>-9.68264637608445</v>
       </c>
       <c r="E26" t="n">
-        <v>0.000000000000000000000356090794367538</v>
+        <v>0.0000000000000000000003573441961612</v>
       </c>
       <c r="F26" t="n">
-        <v>0.000000000000000000209988060293331</v>
+        <v>0.000000000000000000210727195973282</v>
       </c>
       <c r="G26" t="s">
         <v>31</v>
@@ -1354,19 +1354,19 @@
         <v>264.783936280636</v>
       </c>
       <c r="B27" t="n">
-        <v>2.19014730721736</v>
+        <v>2.19014736403873</v>
       </c>
       <c r="C27" t="n">
-        <v>0.208288617632751</v>
+        <v>0.208283540065825</v>
       </c>
       <c r="D27" t="n">
-        <v>10.5149639577472</v>
+        <v>10.5152205659006</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0000000000000000000000000737089839917488</v>
+        <v>0.0000000000000000000000000735086033495087</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0000000000000000000000510258453528967</v>
+        <v>0.0000000000000000000000508871296752555</v>
       </c>
       <c r="G27" t="s">
         <v>32</v>
@@ -1377,19 +1377,19 @@
         <v>51.1459392403024</v>
       </c>
       <c r="B28" t="n">
-        <v>1.89596543238415</v>
+        <v>1.89596541102679</v>
       </c>
       <c r="C28" t="n">
-        <v>0.334033789500674</v>
+        <v>0.334030727609781</v>
       </c>
       <c r="D28" t="n">
-        <v>5.67596899468857</v>
+        <v>5.67602095948993</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0000000137905757634377</v>
+        <v>0.0000000137863894256667</v>
       </c>
       <c r="F28" t="n">
-        <v>0.00000166343596443526</v>
+        <v>0.00000166293100329898</v>
       </c>
       <c r="G28" t="s">
         <v>33</v>
@@ -1400,19 +1400,19 @@
         <v>93.7375117004608</v>
       </c>
       <c r="B29" t="n">
-        <v>-2.13686450701274</v>
+        <v>-2.13686406162334</v>
       </c>
       <c r="C29" t="n">
-        <v>0.198463375071615</v>
+        <v>0.198468805021396</v>
       </c>
       <c r="D29" t="n">
-        <v>-10.7670470999581</v>
+        <v>-10.7667502779239</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0000000000000000000000000049254560250633</v>
+        <v>0.00000000000000000000000000494135620395245</v>
       </c>
       <c r="F29" t="n">
-        <v>0.00000000000000000000000356468685595718</v>
+        <v>0.0000000000000000000000035761942490605</v>
       </c>
       <c r="G29" t="s">
         <v>34</v>
@@ -1423,19 +1423,19 @@
         <v>635.597431692127</v>
       </c>
       <c r="B30" t="n">
-        <v>-2.05686513736594</v>
+        <v>-2.05686530496174</v>
       </c>
       <c r="C30" t="n">
-        <v>0.158732457204121</v>
+        <v>0.158729675928557</v>
       </c>
       <c r="D30" t="n">
-        <v>-12.9580627276558</v>
+        <v>-12.9582908358455</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0000000000000000000000000000000000000211522206845235</v>
+        <v>0.0000000000000000000000000000000000000210894229099443</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0000000000000000000000000000000000306168779762712</v>
+        <v>0.0000000000000000000000000000000000305259810520121</v>
       </c>
       <c r="G30" t="s">
         <v>35</v>
@@ -1446,19 +1446,19 @@
         <v>8370.77697832865</v>
       </c>
       <c r="B31" t="n">
-        <v>-1.05138672089808</v>
+        <v>-1.05138670160618</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0801061350278114</v>
+        <v>0.0801084588078198</v>
       </c>
       <c r="D31" t="n">
-        <v>-13.1249213375861</v>
+        <v>-13.1245403700558</v>
       </c>
       <c r="E31" t="n">
-        <v>0.00000000000000000000000000000000000000237028753617212</v>
+        <v>0.0000000000000000000000000000000000000023822372482883</v>
       </c>
       <c r="F31" t="n">
-        <v>0.00000000000000000000000000000000000377397181509324</v>
+        <v>0.00000000000000000000000000000000000379299814672464</v>
       </c>
       <c r="G31" t="s">
         <v>36</v>
@@ -1469,19 +1469,19 @@
         <v>85.2475378925759</v>
       </c>
       <c r="B32" t="n">
-        <v>1.53414998818525</v>
+        <v>1.53415024655909</v>
       </c>
       <c r="C32" t="n">
-        <v>0.269371974212242</v>
+        <v>0.269368922355899</v>
       </c>
       <c r="D32" t="n">
-        <v>5.69528434675418</v>
+        <v>5.69534983153002</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0000000123166476474368</v>
+        <v>0.0000000123119209888466</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0000014990669548651</v>
+        <v>0.00000149904579799462</v>
       </c>
       <c r="G32" t="s">
         <v>37</v>
@@ -1492,19 +1492,19 @@
         <v>204.50841768509</v>
       </c>
       <c r="B33" t="n">
-        <v>-1.37004892706192</v>
+        <v>-1.37004861723491</v>
       </c>
       <c r="C33" t="n">
-        <v>0.228219436784769</v>
+        <v>0.228213865076486</v>
       </c>
       <c r="D33" t="n">
-        <v>-6.00320878170424</v>
+        <v>-6.00335398892497</v>
       </c>
       <c r="E33" t="n">
-        <v>0.00000000193455594921734</v>
+        <v>0.0000000019328258350981</v>
       </c>
       <c r="F33" t="n">
-        <v>0.000000287869157228397</v>
+        <v>0.000000287611709779737</v>
       </c>
       <c r="G33" t="s">
         <v>38</v>
@@ -1515,19 +1515,19 @@
         <v>100.744231365123</v>
       </c>
       <c r="B34" t="n">
-        <v>2.96472373177385</v>
+        <v>2.96472376618514</v>
       </c>
       <c r="C34" t="n">
-        <v>0.290846419285344</v>
+        <v>0.290841670387607</v>
       </c>
       <c r="D34" t="n">
-        <v>10.1934338372074</v>
+        <v>10.1936003951361</v>
       </c>
       <c r="E34" t="n">
-        <v>0.00000000000000000000000212136043063014</v>
+        <v>0.00000000000000000000000211772785008743</v>
       </c>
       <c r="F34" t="n">
-        <v>0.00000000000000000000140734586568721</v>
+        <v>0.00000000000000000000140493595121217</v>
       </c>
       <c r="G34" t="s">
         <v>39</v>
@@ -1538,19 +1538,19 @@
         <v>127.696605446392</v>
       </c>
       <c r="B35" t="n">
-        <v>-3.06250752675629</v>
+        <v>-3.06250718987228</v>
       </c>
       <c r="C35" t="n">
-        <v>0.260314541111612</v>
+        <v>0.260309591387364</v>
       </c>
       <c r="D35" t="n">
-        <v>-11.7646425500418</v>
+        <v>-11.7648649577225</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0000000000000000000000000000000593772948867906</v>
+        <v>0.0000000000000000000000000000000592210290915595</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0000000000000000000000000000590878305742175</v>
+        <v>0.0000000000000000000000000000589323265747382</v>
       </c>
       <c r="G35" t="s">
         <v>40</v>
@@ -1561,19 +1561,19 @@
         <v>108.03854502188</v>
       </c>
       <c r="B36" t="n">
-        <v>-1.25795836013003</v>
+        <v>-1.25795832319306</v>
       </c>
       <c r="C36" t="n">
-        <v>0.215736411697831</v>
+        <v>0.215737122699906</v>
       </c>
       <c r="D36" t="n">
-        <v>-5.83099695702722</v>
+        <v>-5.83097756867233</v>
       </c>
       <c r="E36" t="n">
-        <v>0.00000000550971895696461</v>
+        <v>0.00000000551035925956496</v>
       </c>
       <c r="F36" t="n">
-        <v>0.000000754763560756219</v>
+        <v>0.000000753973136991014</v>
       </c>
       <c r="G36" t="s">
         <v>41</v>
@@ -1584,19 +1584,19 @@
         <v>1081.42226353696</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.37658836697715</v>
+        <v>-1.37658841999554</v>
       </c>
       <c r="C37" t="n">
-        <v>0.142894089323026</v>
+        <v>0.14289196543924</v>
       </c>
       <c r="D37" t="n">
-        <v>-9.63362706952305</v>
+        <v>-9.63377063058796</v>
       </c>
       <c r="E37" t="n">
-        <v>0.000000000000000000000576575710256711</v>
+        <v>0.000000000000000000000575770438830202</v>
       </c>
       <c r="F37" t="n">
-        <v>0.000000000000000000327865659239548</v>
+        <v>0.000000000000000000327407747394803</v>
       </c>
       <c r="G37" t="s">
         <v>42</v>
@@ -1607,19 +1607,19 @@
         <v>84.3330296604287</v>
       </c>
       <c r="B38" t="n">
-        <v>1.41926682987848</v>
+        <v>1.41926663879356</v>
       </c>
       <c r="C38" t="n">
-        <v>0.335811476803158</v>
+        <v>0.335800556543292</v>
       </c>
       <c r="D38" t="n">
-        <v>4.22637976340043</v>
+        <v>4.22651663655174</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0000237481072228596</v>
+        <v>0.0000237336732256684</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00120037258159483</v>
+        <v>0.00119964300031458</v>
       </c>
       <c r="G38" t="s">
         <v>43</v>
@@ -1630,19 +1630,19 @@
         <v>191.333305944516</v>
       </c>
       <c r="B39" t="n">
-        <v>1.96270554019938</v>
+        <v>1.9627058104106</v>
       </c>
       <c r="C39" t="n">
-        <v>0.232772320202194</v>
+        <v>0.232766583205535</v>
       </c>
       <c r="D39" t="n">
-        <v>8.4318682672171</v>
+        <v>8.43207724829431</v>
       </c>
       <c r="E39" t="n">
-        <v>0.0000000000000000340189812345829</v>
+        <v>0.0000000000000000339582689181398</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0000000000000164136430065767</v>
+        <v>0.0000000000000163843502337764</v>
       </c>
       <c r="G39" t="s">
         <v>44</v>
@@ -1653,19 +1653,19 @@
         <v>108.430344075235</v>
       </c>
       <c r="B40" t="n">
-        <v>1.93727484841215</v>
+        <v>1.93727483233167</v>
       </c>
       <c r="C40" t="n">
-        <v>0.23275552698801</v>
+        <v>0.232754657425924</v>
       </c>
       <c r="D40" t="n">
-        <v>8.32321738384301</v>
+        <v>8.32324840996243</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0000000000000000856072367529364</v>
+        <v>0.0000000000000000855848221754276</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0000000000000378975206013799</v>
+        <v>0.0000000000000378522649632544</v>
       </c>
       <c r="G40" t="s">
         <v>45</v>
@@ -1676,19 +1676,19 @@
         <v>60.4422754951798</v>
       </c>
       <c r="B41" t="n">
-        <v>1.34410361808112</v>
+        <v>1.34410365869374</v>
       </c>
       <c r="C41" t="n">
-        <v>0.34939194160728</v>
+        <v>0.349384542339855</v>
       </c>
       <c r="D41" t="n">
-        <v>3.84697944634311</v>
+        <v>3.84706103393177</v>
       </c>
       <c r="E41" t="n">
-        <v>0.000119582996991535</v>
+        <v>0.000119543197317715</v>
       </c>
       <c r="F41" t="n">
-        <v>0.00470123574839314</v>
+        <v>0.0046996710807226</v>
       </c>
       <c r="G41" t="s">
         <v>46</v>
@@ -1699,19 +1699,19 @@
         <v>583.196745339273</v>
       </c>
       <c r="B42" t="n">
-        <v>-1.2758063764754</v>
+        <v>-1.27580628830243</v>
       </c>
       <c r="C42" t="n">
-        <v>0.149824310271544</v>
+        <v>0.149822574498824</v>
       </c>
       <c r="D42" t="n">
-        <v>-8.51534957286375</v>
+        <v>-8.51544763911692</v>
       </c>
       <c r="E42" t="n">
-        <v>0.000000000000000016608851399774</v>
+        <v>0.0000000000000000165948014100491</v>
       </c>
       <c r="F42" t="n">
-        <v>0.00000000000000881487106624003</v>
+        <v>0.00000000000000880741426836006</v>
       </c>
       <c r="G42" t="s">
         <v>47</v>
@@ -1722,19 +1722,19 @@
         <v>51.5454020090145</v>
       </c>
       <c r="B43" t="n">
-        <v>1.68039202386553</v>
+        <v>1.68039201106918</v>
       </c>
       <c r="C43" t="n">
-        <v>0.307590366960272</v>
+        <v>0.307590115783374</v>
       </c>
       <c r="D43" t="n">
-        <v>5.46308403761736</v>
+        <v>5.4630884571487</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0000000467932938083409</v>
+        <v>0.0000000467921283700978</v>
       </c>
       <c r="F43" t="n">
-        <v>0.00000514507889531577</v>
+        <v>0.00000514037239759954</v>
       </c>
       <c r="G43" t="s">
         <v>48</v>
@@ -1745,19 +1745,19 @@
         <v>56.7888790115642</v>
       </c>
       <c r="B44" t="n">
-        <v>-3.94071640433672</v>
+        <v>-3.94071620206277</v>
       </c>
       <c r="C44" t="n">
-        <v>0.337395072471233</v>
+        <v>0.337398354435135</v>
       </c>
       <c r="D44" t="n">
-        <v>-11.679827969843</v>
+        <v>-11.6797137575263</v>
       </c>
       <c r="E44" t="n">
-        <v>0.000000000000000000000000000000161622293567782</v>
+        <v>0.000000000000000000000000000000161839597490784</v>
       </c>
       <c r="F44" t="n">
-        <v>0.000000000000000000000000000151373538716836</v>
+        <v>0.000000000000000000000000000151577063014604</v>
       </c>
       <c r="G44" t="s">
         <v>49</v>
@@ -1768,19 +1768,19 @@
         <v>59.8249996660037</v>
       </c>
       <c r="B45" t="n">
-        <v>1.60935754018598</v>
+        <v>1.60935759332122</v>
       </c>
       <c r="C45" t="n">
-        <v>0.311184375127484</v>
+        <v>0.311181156392046</v>
       </c>
       <c r="D45" t="n">
-        <v>5.1717170552881</v>
+        <v>5.17177072024775</v>
       </c>
       <c r="E45" t="n">
-        <v>0.000000231952628211483</v>
+        <v>0.000000231886007730263</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0000211037128364756</v>
+        <v>0.00002109765151475</v>
       </c>
       <c r="G45" t="s">
         <v>50</v>
@@ -1791,19 +1791,19 @@
         <v>486.382773500541</v>
       </c>
       <c r="B46" t="n">
-        <v>1.06008128797823</v>
+        <v>1.06008127359453</v>
       </c>
       <c r="C46" t="n">
-        <v>0.179513416335595</v>
+        <v>0.179509393341777</v>
       </c>
       <c r="D46" t="n">
-        <v>5.90530395787488</v>
+        <v>5.90543622180364</v>
       </c>
       <c r="E46" t="n">
-        <v>0.00000000351997142637878</v>
+        <v>0.00000000351714836845478</v>
       </c>
       <c r="F46" t="n">
-        <v>0.000000495973319033655</v>
+        <v>0.000000495575542677319</v>
       </c>
       <c r="G46" t="s">
         <v>51</v>
@@ -1814,19 +1814,19 @@
         <v>52.725275525755</v>
       </c>
       <c r="B47" t="n">
-        <v>-1.088800794081</v>
+        <v>-1.08880059371539</v>
       </c>
       <c r="C47" t="n">
-        <v>0.277467192103819</v>
+        <v>0.277469988987757</v>
       </c>
       <c r="D47" t="n">
-        <v>-3.92407039486531</v>
+        <v>-3.92403011831104</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0000870652762572725</v>
+        <v>0.0000870798416483254</v>
       </c>
       <c r="F47" t="n">
-        <v>0.00365084109084038</v>
+        <v>0.00364950797985938</v>
       </c>
       <c r="G47" t="s">
         <v>52</v>
@@ -1837,19 +1837,19 @@
         <v>61.5508164392515</v>
       </c>
       <c r="B48" t="n">
-        <v>1.73113607831744</v>
+        <v>1.73113639094736</v>
       </c>
       <c r="C48" t="n">
-        <v>0.33428353826355</v>
+        <v>0.334277723406422</v>
       </c>
       <c r="D48" t="n">
-        <v>5.1786459103248</v>
+        <v>5.17873692959972</v>
       </c>
       <c r="E48" t="n">
-        <v>0.000000223502229115377</v>
+        <v>0.000000223393226911725</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0000205699566010117</v>
+        <v>0.0000205599246178525</v>
       </c>
       <c r="G48" t="s">
         <v>53</v>
@@ -1860,19 +1860,19 @@
         <v>292.943517964495</v>
       </c>
       <c r="B49" t="n">
-        <v>1.14367436431805</v>
+        <v>1.14367426429324</v>
       </c>
       <c r="C49" t="n">
-        <v>0.138108830202112</v>
+        <v>0.138110860029009</v>
       </c>
       <c r="D49" t="n">
-        <v>8.28096482060106</v>
+        <v>8.2808423903306</v>
       </c>
       <c r="E49" t="n">
-        <v>0.000000000000000122181282982572</v>
+        <v>0.000000000000000122306976239523</v>
       </c>
       <c r="F49" t="n">
-        <v>0.0000000000000525775780445542</v>
+        <v>0.0000000000000526316669104239</v>
       </c>
       <c r="G49" t="s">
         <v>54</v>
@@ -1883,19 +1883,19 @@
         <v>95.4229952380182</v>
       </c>
       <c r="B50" t="n">
-        <v>-7.55521776583524</v>
+        <v>-7.55521817766787</v>
       </c>
       <c r="C50" t="n">
-        <v>0.668900289833191</v>
+        <v>0.668902490741008</v>
       </c>
       <c r="D50" t="n">
-        <v>-11.2949835433908</v>
+        <v>-11.2949469948874</v>
       </c>
       <c r="E50" t="n">
-        <v>0.0000000000000000000000000000138930076968824</v>
+        <v>0.0000000000000000000000000000138987884050042</v>
       </c>
       <c r="F50" t="n">
-        <v>0.0000000000000000000000000116423404499874</v>
+        <v>0.0000000000000000000000000116471846833936</v>
       </c>
       <c r="G50" t="s">
         <v>55</v>
@@ -1906,19 +1906,19 @@
         <v>163.738012785676</v>
       </c>
       <c r="B51" t="n">
-        <v>-2.26434382348164</v>
+        <v>-2.26434381453938</v>
       </c>
       <c r="C51" t="n">
-        <v>0.196408714179131</v>
+        <v>0.196408789110402</v>
       </c>
       <c r="D51" t="n">
-        <v>-11.5287340123641</v>
+        <v>-11.5287295685459</v>
       </c>
       <c r="E51" t="n">
-        <v>0.000000000000000000000000000000945234421873294</v>
+        <v>0.000000000000000000000000000000945283208052196</v>
       </c>
       <c r="F51" t="n">
-        <v>0.000000000000000000000000000836112359170366</v>
+        <v>0.000000000000000000000000000836155513255948</v>
       </c>
       <c r="G51" t="s">
         <v>56</v>
@@ -1929,19 +1929,19 @@
         <v>69.2232553988309</v>
       </c>
       <c r="B52" t="n">
-        <v>-5.79520515213206</v>
+        <v>-5.79520522109589</v>
       </c>
       <c r="C52" t="n">
-        <v>0.484013764636946</v>
+        <v>0.484013334467383</v>
       </c>
       <c r="D52" t="n">
-        <v>-11.9732238534145</v>
+        <v>-11.9732346371677</v>
       </c>
       <c r="E52" t="n">
-        <v>0.00000000000000000000000000000000490836699724711</v>
+        <v>0.00000000000000000000000000000000490772892718247</v>
       </c>
       <c r="F52" t="n">
-        <v>0.00000000000000000000000000000558221566644061</v>
+        <v>0.00000000000000000000000000000558148999847137</v>
       </c>
       <c r="G52" t="s">
         <v>57</v>
@@ -1952,19 +1952,19 @@
         <v>68.0530153779782</v>
       </c>
       <c r="B53" t="n">
-        <v>2.27627415011187</v>
+        <v>2.27627427499524</v>
       </c>
       <c r="C53" t="n">
-        <v>0.268865112844235</v>
+        <v>0.268866412069487</v>
       </c>
       <c r="D53" t="n">
-        <v>8.46623098858725</v>
+        <v>8.46619054226435</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0000000000000000253461271048534</v>
+        <v>0.0000000000000000253549257558961</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0000000000000130180979278541</v>
+        <v>0.0000000000000130226170285606</v>
       </c>
       <c r="G53" t="s">
         <v>58</v>
@@ -1975,19 +1975,19 @@
         <v>57.31562386548</v>
       </c>
       <c r="B54" t="n">
-        <v>1.69337476054297</v>
+        <v>1.6933756534712</v>
       </c>
       <c r="C54" t="n">
-        <v>0.471072289037267</v>
+        <v>0.471053703630177</v>
       </c>
       <c r="D54" t="n">
-        <v>3.59472378221128</v>
+        <v>3.59486750750752</v>
       </c>
       <c r="E54" t="n">
-        <v>0.000324735919641773</v>
+        <v>0.00032455670398177</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0104896787378288</v>
+        <v>0.0104930004295231</v>
       </c>
       <c r="G54" t="s">
         <v>59</v>
@@ -1998,19 +1998,19 @@
         <v>281.879678022693</v>
       </c>
       <c r="B55" t="n">
-        <v>-1.45507293322301</v>
+        <v>-1.45507292615028</v>
       </c>
       <c r="C55" t="n">
-        <v>0.150147009331997</v>
+        <v>0.150148140578941</v>
       </c>
       <c r="D55" t="n">
-        <v>-9.69098844989736</v>
+        <v>-9.69091538889396</v>
       </c>
       <c r="E55" t="n">
-        <v>0.000000000000000000000329325813608605</v>
+        <v>0.000000000000000000000329561503241334</v>
       </c>
       <c r="F55" t="n">
-        <v>0.000000000000000000201674061702931</v>
+        <v>0.00000000000000000020181839440802</v>
       </c>
       <c r="G55" t="s">
         <v>60</v>
@@ -2021,19 +2021,19 @@
         <v>62.5686560719231</v>
       </c>
       <c r="B56" t="n">
-        <v>-1.16958883716655</v>
+        <v>-1.16958884049603</v>
       </c>
       <c r="C56" t="n">
-        <v>0.275933901887106</v>
+        <v>0.275934052330925</v>
       </c>
       <c r="D56" t="n">
-        <v>-4.23865581274269</v>
+        <v>-4.23865351382348</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0000224862093016242</v>
+        <v>0.0000224864395276693</v>
       </c>
       <c r="F56" t="n">
-        <v>0.00114020835828172</v>
+        <v>0.00114022003235526</v>
       </c>
       <c r="G56" t="s">
         <v>61</v>
@@ -2044,19 +2044,19 @@
         <v>1004.59669967681</v>
       </c>
       <c r="B57" t="n">
-        <v>-1.19816865703506</v>
+        <v>-1.19816858205053</v>
       </c>
       <c r="C57" t="n">
-        <v>0.142997883489717</v>
+        <v>0.142995756341931</v>
       </c>
       <c r="D57" t="n">
-        <v>-8.37892581201194</v>
+        <v>-8.37904992918442</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0000000000000000534129266300786</v>
+        <v>0.0000000000000000533566380160263</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0000000000000250129593471797</v>
+        <v>0.0000000000000249865997203286</v>
       </c>
       <c r="G57" t="s">
         <v>62</v>
@@ -2067,19 +2067,19 @@
         <v>54.6482819922743</v>
       </c>
       <c r="B58" t="n">
-        <v>2.20312397417773</v>
+        <v>2.20312397491421</v>
       </c>
       <c r="C58" t="n">
-        <v>0.514496004389901</v>
+        <v>0.514473463984859</v>
       </c>
       <c r="D58" t="n">
-        <v>4.2821012318458</v>
+        <v>4.2822888431405</v>
       </c>
       <c r="E58" t="n">
-        <v>0.0000185136715753528</v>
+        <v>0.0000184980642711428</v>
       </c>
       <c r="F58" t="n">
-        <v>0.000969653548759105</v>
+        <v>0.000968836116201106</v>
       </c>
       <c r="G58" t="s">
         <v>63</v>
@@ -2090,19 +2090,19 @@
         <v>64.7467529031255</v>
       </c>
       <c r="B59" t="n">
-        <v>1.23917381971217</v>
+        <v>1.23917375948506</v>
       </c>
       <c r="C59" t="n">
-        <v>0.340898570294434</v>
+        <v>0.340890749545011</v>
       </c>
       <c r="D59" t="n">
-        <v>3.63502204964338</v>
+        <v>3.63510526800448</v>
       </c>
       <c r="E59" t="n">
-        <v>0.000277956861341282</v>
+        <v>0.00027786715082166</v>
       </c>
       <c r="F59" t="n">
-        <v>0.00922006072140812</v>
+        <v>0.00921708494871348</v>
       </c>
       <c r="G59" t="s">
         <v>64</v>
@@ -2113,19 +2113,19 @@
         <v>101.95532974134</v>
       </c>
       <c r="B60" t="n">
-        <v>-1.05935409858241</v>
+        <v>-1.05935396006618</v>
       </c>
       <c r="C60" t="n">
-        <v>0.26069245964755</v>
+        <v>0.260688444525014</v>
       </c>
       <c r="D60" t="n">
-        <v>-4.06361618596347</v>
+        <v>-4.06367824241834</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0000483182538465149</v>
+        <v>0.0000483054032000158</v>
       </c>
       <c r="F60" t="n">
-        <v>0.00222347756573471</v>
+        <v>0.00222288621315217</v>
       </c>
       <c r="G60" t="s">
         <v>65</v>
@@ -2136,19 +2136,19 @@
         <v>52.270549866692</v>
       </c>
       <c r="B61" t="n">
-        <v>1.29999043585408</v>
+        <v>1.29999016226921</v>
       </c>
       <c r="C61" t="n">
-        <v>0.355973240265527</v>
+        <v>0.355967078103315</v>
       </c>
       <c r="D61" t="n">
-        <v>3.65193303542816</v>
+        <v>3.65199548563844</v>
       </c>
       <c r="E61" t="n">
-        <v>0.000260273762028938</v>
+        <v>0.000260210460337357</v>
       </c>
       <c r="F61" t="n">
-        <v>0.00884135210113377</v>
+        <v>0.00884385282335973</v>
       </c>
       <c r="G61" t="s">
         <v>66</v>
@@ -2159,19 +2159,19 @@
         <v>142.197666437416</v>
       </c>
       <c r="B62" t="n">
-        <v>-1.48882761588297</v>
+        <v>-1.48882760976979</v>
       </c>
       <c r="C62" t="n">
-        <v>0.257069356576633</v>
+        <v>0.257062821944992</v>
       </c>
       <c r="D62" t="n">
-        <v>-5.79154060098621</v>
+        <v>-5.79168780030114</v>
       </c>
       <c r="E62" t="n">
-        <v>0.00000000697436940979547</v>
+        <v>0.00000000696825829468452</v>
       </c>
       <c r="F62" t="n">
-        <v>0.000000917734791262508</v>
+        <v>0.000000916930649322041</v>
       </c>
       <c r="G62" t="s">
         <v>67</v>
@@ -2182,19 +2182,19 @@
         <v>378.274757795154</v>
       </c>
       <c r="B63" t="n">
-        <v>1.19898698231286</v>
+        <v>1.1989868244721</v>
       </c>
       <c r="C63" t="n">
-        <v>0.244482311941425</v>
+        <v>0.244473278322481</v>
       </c>
       <c r="D63" t="n">
-        <v>4.90418702601323</v>
+        <v>4.90436759673399</v>
       </c>
       <c r="E63" t="n">
-        <v>0.000000938150715859739</v>
+        <v>0.000000937288182549272</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0000714700272627692</v>
+        <v>0.0000714043179069354</v>
       </c>
       <c r="G63" t="s">
         <v>68</v>
@@ -2205,19 +2205,19 @@
         <v>277.896199205694</v>
       </c>
       <c r="B64" t="n">
-        <v>1.09533968187963</v>
+        <v>1.09533961931193</v>
       </c>
       <c r="C64" t="n">
-        <v>0.295562235313003</v>
+        <v>0.29554973404869</v>
       </c>
       <c r="D64" t="n">
-        <v>3.70595276057393</v>
+        <v>3.70610930453916</v>
       </c>
       <c r="E64" t="n">
-        <v>0.00021059755248705</v>
+        <v>0.0002104674961354</v>
       </c>
       <c r="F64" t="n">
-        <v>0.00760347898117645</v>
+        <v>0.0075987833865484</v>
       </c>
       <c r="G64" t="s">
         <v>69</v>
@@ -2228,19 +2228,19 @@
         <v>90.2702229666148</v>
       </c>
       <c r="B65" t="n">
-        <v>2.24071520980866</v>
+        <v>2.24071545288914</v>
       </c>
       <c r="C65" t="n">
-        <v>0.326999908007746</v>
+        <v>0.326990276556166</v>
       </c>
       <c r="D65" t="n">
-        <v>6.85234201887172</v>
+        <v>6.85254459700809</v>
       </c>
       <c r="E65" t="n">
-        <v>0.0000000000072650600697789</v>
+        <v>0.00000000000725477585072809</v>
       </c>
       <c r="F65" t="n">
-        <v>0.00000000165248980615742</v>
+        <v>0.00000000165015058707561</v>
       </c>
       <c r="G65" t="s">
         <v>70</v>
@@ -2251,19 +2251,19 @@
         <v>107.220681398004</v>
       </c>
       <c r="B66" t="n">
-        <v>-1.22257644112265</v>
+        <v>-1.22257637828133</v>
       </c>
       <c r="C66" t="n">
-        <v>0.262088540413973</v>
+        <v>0.262083767746057</v>
       </c>
       <c r="D66" t="n">
-        <v>-4.66474588775066</v>
+        <v>-4.66483059517798</v>
       </c>
       <c r="E66" t="n">
-        <v>0.00000308998645486227</v>
+        <v>0.00000308871387967861</v>
       </c>
       <c r="F66" t="n">
-        <v>0.000201634280058677</v>
+        <v>0.000201551239312471</v>
       </c>
       <c r="G66" t="s">
         <v>71</v>
@@ -2274,19 +2274,19 @@
         <v>274.489839912433</v>
       </c>
       <c r="B67" t="n">
-        <v>1.10232518314036</v>
+        <v>1.10232546263878</v>
       </c>
       <c r="C67" t="n">
-        <v>0.246172489301807</v>
+        <v>0.246164220525272</v>
       </c>
       <c r="D67" t="n">
-        <v>4.47785691352747</v>
+        <v>4.47800846234522</v>
       </c>
       <c r="E67" t="n">
-        <v>0.00000753961067759122</v>
+        <v>0.00000753426156236937</v>
       </c>
       <c r="F67" t="n">
-        <v>0.000442972993389695</v>
+        <v>0.000442658718066587</v>
       </c>
       <c r="G67" t="s">
         <v>72</v>
@@ -2297,19 +2297,19 @@
         <v>332.256566441655</v>
       </c>
       <c r="B68" t="n">
-        <v>-1.65140559483778</v>
+        <v>-1.65140570494185</v>
       </c>
       <c r="C68" t="n">
-        <v>0.271510266847254</v>
+        <v>0.271499361215911</v>
       </c>
       <c r="D68" t="n">
-        <v>-6.08229520752094</v>
+        <v>-6.08253992770378</v>
       </c>
       <c r="E68" t="n">
-        <v>0.00000000118474172910325</v>
+        <v>0.00000000118293425019004</v>
       </c>
       <c r="F68" t="n">
-        <v>0.000000188634578107819</v>
+        <v>0.000000188346791315258</v>
       </c>
       <c r="G68" t="s">
         <v>73</v>
@@ -2326,13 +2326,13 @@
         <v>0.808075105001968</v>
       </c>
       <c r="D69" t="n">
-        <v>5.92170748894356</v>
+        <v>5.92170748894357</v>
       </c>
       <c r="E69" t="n">
-        <v>0.00000000318615976368185</v>
+        <v>0.00000000318615976368173</v>
       </c>
       <c r="F69" t="n">
-        <v>0.000000457027349165248</v>
+        <v>0.00000045702734916523</v>
       </c>
       <c r="G69" t="s">
         <v>74</v>
@@ -2343,19 +2343,19 @@
         <v>66.6023892446988</v>
       </c>
       <c r="B70" t="n">
-        <v>-2.17362210866823</v>
+        <v>-2.1736220857366</v>
       </c>
       <c r="C70" t="n">
-        <v>0.279492712298544</v>
+        <v>0.279493031534942</v>
       </c>
       <c r="D70" t="n">
-        <v>-7.77702606551844</v>
+        <v>-7.77701710056714</v>
       </c>
       <c r="E70" t="n">
-        <v>0.00000000000000742493124860936</v>
+        <v>0.00000000000000742545723501398</v>
       </c>
       <c r="F70" t="n">
-        <v>0.00000000000262710567423018</v>
+        <v>0.00000000000262729177990872</v>
       </c>
       <c r="G70" t="s">
         <v>75</v>
@@ -2366,19 +2366,19 @@
         <v>196.303774044731</v>
       </c>
       <c r="B71" t="n">
-        <v>1.11446447034203</v>
+        <v>1.11446445816354</v>
       </c>
       <c r="C71" t="n">
-        <v>0.315615650847755</v>
+        <v>0.315602765466978</v>
       </c>
       <c r="D71" t="n">
-        <v>3.53108113412165</v>
+        <v>3.53122526196668</v>
       </c>
       <c r="E71" t="n">
-        <v>0.000413864778829543</v>
+        <v>0.000413639318730105</v>
       </c>
       <c r="F71" t="n">
-        <v>0.0127457543685183</v>
+        <v>0.0127388108952045</v>
       </c>
       <c r="G71" t="s">
         <v>76</v>
@@ -2389,19 +2389,19 @@
         <v>519.190330332328</v>
       </c>
       <c r="B72" t="n">
-        <v>1.10941211265179</v>
+        <v>1.10941197676593</v>
       </c>
       <c r="C72" t="n">
-        <v>0.192175394446539</v>
+        <v>0.192170094537083</v>
       </c>
       <c r="D72" t="n">
-        <v>5.77291445581196</v>
+        <v>5.77307296142195</v>
       </c>
       <c r="E72" t="n">
-        <v>0.00000000779120018091134</v>
+        <v>0.00000000778387160623517</v>
       </c>
       <c r="F72" t="n">
-        <v>0.00000100940771050294</v>
+        <v>0.00000100888770742758</v>
       </c>
       <c r="G72" t="s">
         <v>77</v>
@@ -2412,19 +2412,19 @@
         <v>200.946108293183</v>
       </c>
       <c r="B73" t="n">
-        <v>1.21282390537619</v>
+        <v>1.21282386527637</v>
       </c>
       <c r="C73" t="n">
-        <v>0.157527803160719</v>
+        <v>0.157529884290666</v>
       </c>
       <c r="D73" t="n">
-        <v>7.69911013193521</v>
+        <v>7.6990081643082</v>
       </c>
       <c r="E73" t="n">
-        <v>0.0000000000000137017042364728</v>
+        <v>0.0000000000000137126409931242</v>
       </c>
       <c r="F73" t="n">
-        <v>0.00000000000464167095432169</v>
+        <v>0.00000000000464537595516007</v>
       </c>
       <c r="G73" t="s">
         <v>78</v>
@@ -2435,19 +2435,19 @@
         <v>132.935874312163</v>
       </c>
       <c r="B74" t="n">
-        <v>-1.92162249156259</v>
+        <v>-1.92162230638247</v>
       </c>
       <c r="C74" t="n">
-        <v>0.265251050970092</v>
+        <v>0.265244392141188</v>
       </c>
       <c r="D74" t="n">
-        <v>-7.24454242324289</v>
+        <v>-7.24472359573809</v>
       </c>
       <c r="E74" t="n">
-        <v>0.000000000000433901584779816</v>
+        <v>0.000000000000433321992029534</v>
       </c>
       <c r="F74" t="n">
-        <v>0.00000000011142872633652</v>
+        <v>0.000000000111279883178939</v>
       </c>
       <c r="G74" t="s">
         <v>79</v>
@@ -2458,19 +2458,19 @@
         <v>461.284863486414</v>
       </c>
       <c r="B75" t="n">
-        <v>-1.51457181349827</v>
+        <v>-1.51457187061751</v>
       </c>
       <c r="C75" t="n">
-        <v>0.165471208432994</v>
+        <v>0.165468707658962</v>
       </c>
       <c r="D75" t="n">
-        <v>-9.15308365631217</v>
+        <v>-9.15322233457644</v>
       </c>
       <c r="E75" t="n">
-        <v>0.0000000000000000000553311037933738</v>
+        <v>0.0000000000000000000552600958241581</v>
       </c>
       <c r="F75" t="n">
-        <v>0.0000000000000000303786839516586</v>
+        <v>0.0000000000000000303396981280085</v>
       </c>
       <c r="G75" t="s">
         <v>80</v>
@@ -2481,19 +2481,19 @@
         <v>75.7692658308865</v>
       </c>
       <c r="B76" t="n">
-        <v>1.50906512122116</v>
+        <v>1.50906570536114</v>
       </c>
       <c r="C76" t="n">
-        <v>0.351033957566108</v>
+        <v>0.351024145072529</v>
       </c>
       <c r="D76" t="n">
-        <v>4.29891493029407</v>
+        <v>4.29903676583085</v>
       </c>
       <c r="E76" t="n">
-        <v>0.0000171636330713173</v>
+        <v>0.0000171542017204156</v>
       </c>
       <c r="F76" t="n">
-        <v>0.000913977811911418</v>
+        <v>0.00091347558459016</v>
       </c>
       <c r="G76" t="s">
         <v>81</v>
@@ -2504,19 +2504,19 @@
         <v>1101.94850237211</v>
       </c>
       <c r="B77" t="n">
-        <v>1.04331652809452</v>
+        <v>1.04331654446473</v>
       </c>
       <c r="C77" t="n">
-        <v>0.197339232286672</v>
+        <v>0.197332452250088</v>
       </c>
       <c r="D77" t="n">
-        <v>5.28691895678864</v>
+        <v>5.28710069007045</v>
       </c>
       <c r="E77" t="n">
-        <v>0.000000124393716688382</v>
+        <v>0.000000124270243635924</v>
       </c>
       <c r="F77" t="n">
-        <v>0.0000122259059081013</v>
+        <v>0.000012213770488711</v>
       </c>
       <c r="G77" t="s">
         <v>82</v>
@@ -2527,19 +2527,19 @@
         <v>68.0987555865034</v>
       </c>
       <c r="B78" t="n">
-        <v>1.25097025432292</v>
+        <v>1.2509706057776</v>
       </c>
       <c r="C78" t="n">
-        <v>0.389766819804551</v>
+        <v>0.389752373929273</v>
       </c>
       <c r="D78" t="n">
-        <v>3.20953501108746</v>
+        <v>3.20965487179973</v>
       </c>
       <c r="E78" t="n">
-        <v>0.0013294985422748</v>
+        <v>0.00132894433185962</v>
       </c>
       <c r="F78" t="n">
-        <v>0.0324500490268083</v>
+        <v>0.0324531467053203</v>
       </c>
       <c r="G78" t="s">
         <v>83</v>
@@ -2550,19 +2550,19 @@
         <v>103.151771730527</v>
       </c>
       <c r="B79" t="n">
-        <v>-1.21259158052678</v>
+        <v>-1.21259151803846</v>
       </c>
       <c r="C79" t="n">
-        <v>0.259911160773024</v>
+        <v>0.259907167716347</v>
       </c>
       <c r="D79" t="n">
-        <v>-4.66540789137454</v>
+        <v>-4.66547932745679</v>
       </c>
       <c r="E79" t="n">
-        <v>0.00000308005443226571</v>
+        <v>0.00000307898451107769</v>
       </c>
       <c r="F79" t="n">
-        <v>0.000201634280058677</v>
+        <v>0.000201551239312471</v>
       </c>
       <c r="G79" t="s">
         <v>84</v>
@@ -2573,19 +2573,19 @@
         <v>192.63399554599</v>
       </c>
       <c r="B80" t="n">
-        <v>-1.10643917384685</v>
+        <v>-1.10643901945404</v>
       </c>
       <c r="C80" t="n">
-        <v>0.225564387605411</v>
+        <v>0.225559554749241</v>
       </c>
       <c r="D80" t="n">
-        <v>-4.90520327961696</v>
+        <v>-4.90530769438739</v>
       </c>
       <c r="E80" t="n">
-        <v>0.000000933306303963039</v>
+        <v>0.000000932809932450277</v>
       </c>
       <c r="F80" t="n">
-        <v>0.0000714428027485553</v>
+        <v>0.0000714043179069354</v>
       </c>
       <c r="G80" t="s">
         <v>85</v>
@@ -2596,19 +2596,19 @@
         <v>73.1662889957929</v>
       </c>
       <c r="B81" t="n">
-        <v>1.12903547200976</v>
+        <v>1.12903577497755</v>
       </c>
       <c r="C81" t="n">
-        <v>0.308826382693189</v>
+        <v>0.308820581574487</v>
       </c>
       <c r="D81" t="n">
-        <v>3.65589060806189</v>
+        <v>3.6559602641161</v>
       </c>
       <c r="E81" t="n">
-        <v>0.000256290635574976</v>
+        <v>0.000256221044372964</v>
       </c>
       <c r="F81" t="n">
-        <v>0.00877561182715004</v>
+        <v>0.00877322896452974</v>
       </c>
       <c r="G81" t="s">
         <v>86</v>
@@ -2619,19 +2619,19 @@
         <v>351.890563980539</v>
       </c>
       <c r="B82" t="n">
-        <v>-8.95505804558056</v>
+        <v>-8.95505795958088</v>
       </c>
       <c r="C82" t="n">
-        <v>0.571298896632222</v>
+        <v>0.571297869750615</v>
       </c>
       <c r="D82" t="n">
-        <v>-15.6749087008048</v>
+        <v>-15.6749367251973</v>
       </c>
       <c r="E82" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000224547427158926</v>
+        <v>0.000000000000000000000000000000000000000000000000000000224448411506804</v>
       </c>
       <c r="F82" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000893811033806106</v>
+        <v>0.000000000000000000000000000000000000000000000000000893416902002832</v>
       </c>
       <c r="G82" t="s">
         <v>87</v>
@@ -2642,19 +2642,19 @@
         <v>95.6240212539047</v>
       </c>
       <c r="B83" t="n">
-        <v>-4.47556835052205</v>
+        <v>-4.47556812543562</v>
       </c>
       <c r="C83" t="n">
-        <v>0.327916372827286</v>
+        <v>0.327913325430595</v>
       </c>
       <c r="D83" t="n">
-        <v>-13.6485052939987</v>
+        <v>-13.6486314472234</v>
       </c>
       <c r="E83" t="n">
-        <v>0.00000000000000000000000000000000000000000206061844104962</v>
+        <v>0.00000000000000000000000000000000000000000205705468395926</v>
       </c>
       <c r="F83" t="n">
-        <v>0.00000000000000000000000000000000000000410114585229901</v>
+        <v>0.00000000000000000000000000000000000000409405308474992</v>
       </c>
       <c r="G83" t="s">
         <v>88</v>
@@ -2665,19 +2665,19 @@
         <v>372.132930903426</v>
       </c>
       <c r="B84" t="n">
-        <v>5.84171000722159</v>
+        <v>5.84170979411422</v>
       </c>
       <c r="C84" t="n">
-        <v>0.25209081417793</v>
+        <v>0.252085959183725</v>
       </c>
       <c r="D84" t="n">
-        <v>23.1730379636063</v>
+        <v>23.1734834142693</v>
       </c>
       <c r="E84" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000851770888269744</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000843007524790766</v>
       </c>
       <c r="F84" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000678094804151543</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000671118290485929</v>
       </c>
       <c r="G84" t="s">
         <v>89</v>
@@ -2688,19 +2688,19 @@
         <v>134.94161067392</v>
       </c>
       <c r="B85" t="n">
-        <v>-6.37236591607607</v>
+        <v>-6.37236564028817</v>
       </c>
       <c r="C85" t="n">
-        <v>0.414619368099562</v>
+        <v>0.414617702801719</v>
       </c>
       <c r="D85" t="n">
-        <v>-15.3691949927093</v>
+        <v>-15.3692560573941</v>
       </c>
       <c r="E85" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000263421822237262</v>
+        <v>0.0000000000000000000000000000000000000000000000000000263173675411607</v>
       </c>
       <c r="F85" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000838840450732336</v>
+        <v>0.0000000000000000000000000000000000000000000000000838050251980721</v>
       </c>
       <c r="G85" t="s">
         <v>90</v>
@@ -2711,19 +2711,19 @@
         <v>285.430477483444</v>
       </c>
       <c r="B86" t="n">
-        <v>-1.88504825021185</v>
+        <v>-1.88504822777448</v>
       </c>
       <c r="C86" t="n">
-        <v>0.15790094659836</v>
+        <v>0.15790121142018</v>
       </c>
       <c r="D86" t="n">
-        <v>-11.9381694082347</v>
+        <v>-11.9381492442024</v>
       </c>
       <c r="E86" t="n">
-        <v>0.00000000000000000000000000000000748524674406932</v>
+        <v>0.00000000000000000000000000000000748706129465815</v>
       </c>
       <c r="F86" t="n">
-        <v>0.00000000000000000000000000000794533991060478</v>
+        <v>0.0000000000000000000000000000079472659955698</v>
       </c>
       <c r="G86" t="s">
         <v>91</v>
@@ -2734,19 +2734,19 @@
         <v>159.071274127276</v>
       </c>
       <c r="B87" t="n">
-        <v>3.26117466219232</v>
+        <v>3.26117467143012</v>
       </c>
       <c r="C87" t="n">
-        <v>0.234902268263376</v>
+        <v>0.234899404098434</v>
       </c>
       <c r="D87" t="n">
-        <v>13.8831126932152</v>
+        <v>13.8832820114926</v>
       </c>
       <c r="E87" t="n">
-        <v>0.0000000000000000000000000000000000000000000801847172653807</v>
+        <v>0.0000000000000000000000000000000000000000000799954843407919</v>
       </c>
       <c r="F87" t="n">
-        <v>0.000000000000000000000000000000000000000182385866899913</v>
+        <v>0.000000000000000000000000000000000000000181955443096298</v>
       </c>
       <c r="G87" t="s">
         <v>92</v>
@@ -2757,19 +2757,19 @@
         <v>996.65960417238</v>
       </c>
       <c r="B88" t="n">
-        <v>3.1751147545012</v>
+        <v>3.1751147052609</v>
       </c>
       <c r="C88" t="n">
-        <v>0.210668252483228</v>
+        <v>0.210660925496793</v>
       </c>
       <c r="D88" t="n">
-        <v>15.0716337989939</v>
+        <v>15.0721577709447</v>
       </c>
       <c r="E88" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000248881431166691</v>
+        <v>0.00000000000000000000000000000000000000000000000000246915182528815</v>
       </c>
       <c r="F88" t="n">
-        <v>0.00000000000000000000000000000000000000000000000660448357839343</v>
+        <v>0.00000000000000000000000000000000000000000000000655230589370633</v>
       </c>
       <c r="G88" t="s">
         <v>93</v>
@@ -2780,19 +2780,19 @@
         <v>3319.74037422825</v>
       </c>
       <c r="B89" t="n">
-        <v>-5.090864404444</v>
+        <v>-5.09086487068305</v>
       </c>
       <c r="C89" t="n">
-        <v>0.168901381549369</v>
+        <v>0.168895974213965</v>
       </c>
       <c r="D89" t="n">
-        <v>-30.1410465547671</v>
+        <v>-30.1420143042232</v>
       </c>
       <c r="E89" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000140538713454065</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000136494115688403</v>
       </c>
       <c r="F89" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000223765739561562</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000217325930999074</v>
       </c>
       <c r="G89" t="s">
         <v>94</v>
@@ -2803,19 +2803,19 @@
         <v>275.623092034311</v>
       </c>
       <c r="B90" t="n">
-        <v>-5.39678240484157</v>
+        <v>-5.39678303277092</v>
       </c>
       <c r="C90" t="n">
-        <v>0.244488842711776</v>
+        <v>0.24448703739622</v>
       </c>
       <c r="D90" t="n">
-        <v>-22.0737369647732</v>
+        <v>-22.0739025277026</v>
       </c>
       <c r="E90" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000056521525590966</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000563149179943528</v>
       </c>
       <c r="F90" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000299978576819787</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000298882041435362</v>
       </c>
       <c r="G90" t="s">
         <v>95</v>
@@ -2826,19 +2826,19 @@
         <v>349.239133179641</v>
       </c>
       <c r="B91" t="n">
-        <v>-1.30193674828326</v>
+        <v>-1.30193708492269</v>
       </c>
       <c r="C91" t="n">
-        <v>0.242200679157792</v>
+        <v>0.24219191899092</v>
       </c>
       <c r="D91" t="n">
-        <v>-5.37544631505783</v>
+        <v>-5.37564213681094</v>
       </c>
       <c r="E91" t="n">
-        <v>0.0000000763932117719884</v>
+        <v>0.0000000763102245860229</v>
       </c>
       <c r="F91" t="n">
-        <v>0.00000800218893311579</v>
+        <v>0.0000079934960253859</v>
       </c>
       <c r="G91" t="s">
         <v>96</v>
@@ -2849,19 +2849,19 @@
         <v>88.2009272116187</v>
       </c>
       <c r="B92" t="n">
-        <v>1.23702585582094</v>
+        <v>1.23702545116943</v>
       </c>
       <c r="C92" t="n">
-        <v>0.328456246197947</v>
+        <v>0.328446348064357</v>
       </c>
       <c r="D92" t="n">
-        <v>3.76618155428664</v>
+        <v>3.76629382077052</v>
       </c>
       <c r="E92" t="n">
-        <v>0.000165763273206428</v>
+        <v>0.000165688790561865</v>
       </c>
       <c r="F92" t="n">
-        <v>0.00615217444287354</v>
+        <v>0.00614941007768301</v>
       </c>
       <c r="G92" t="s">
         <v>97</v>
@@ -2872,19 +2872,19 @@
         <v>385.745062332128</v>
       </c>
       <c r="B93" t="n">
-        <v>-1.19818010368871</v>
+        <v>-1.19818010461435</v>
       </c>
       <c r="C93" t="n">
-        <v>0.159909210755146</v>
+        <v>0.159907638370429</v>
       </c>
       <c r="D93" t="n">
-        <v>-7.49287735228315</v>
+        <v>-7.49295103613966</v>
       </c>
       <c r="E93" t="n">
-        <v>0.0000000000000673798596964092</v>
+        <v>0.000000000000067342028580102</v>
       </c>
       <c r="F93" t="n">
-        <v>0.0000000000202419269072873</v>
+        <v>0.0000000000202305618689129</v>
       </c>
       <c r="G93" t="s">
         <v>98</v>
@@ -2895,19 +2895,19 @@
         <v>93.7906922500095</v>
       </c>
       <c r="B94" t="n">
-        <v>-1.06977753204982</v>
+        <v>-1.06977770377706</v>
       </c>
       <c r="C94" t="n">
-        <v>0.19675701639151</v>
+        <v>0.196761617640871</v>
       </c>
       <c r="D94" t="n">
-        <v>-5.43704896358645</v>
+        <v>-5.43692269154657</v>
       </c>
       <c r="E94" t="n">
-        <v>0.0000000541702558214898</v>
+        <v>0.0000000542086440324391</v>
       </c>
       <c r="F94" t="n">
-        <v>0.0000058276946837146</v>
+        <v>0.00000583182452894929</v>
       </c>
       <c r="G94" t="s">
         <v>99</v>
@@ -2918,19 +2918,19 @@
         <v>52.9275514675909</v>
       </c>
       <c r="B95" t="n">
-        <v>3.45750147471822</v>
+        <v>3.45750089045931</v>
       </c>
       <c r="C95" t="n">
-        <v>0.466022112291829</v>
+        <v>0.466004812524332</v>
       </c>
       <c r="D95" t="n">
-        <v>7.41917901216045</v>
+        <v>7.4194531848934</v>
       </c>
       <c r="E95" t="n">
-        <v>0.000000000000117848541139</v>
+        <v>0.000000000000117604859511583</v>
       </c>
       <c r="F95" t="n">
-        <v>0.0000000000341160813093665</v>
+        <v>0.0000000000340455376935167</v>
       </c>
       <c r="G95" t="s">
         <v>100</v>
@@ -2941,19 +2941,19 @@
         <v>99.1023155389652</v>
       </c>
       <c r="B96" t="n">
-        <v>-1.12595482928199</v>
+        <v>-1.1259549330556</v>
       </c>
       <c r="C96" t="n">
-        <v>0.270464810658416</v>
+        <v>0.270460205940243</v>
       </c>
       <c r="D96" t="n">
-        <v>-4.16303631714965</v>
+        <v>-4.16310757858542</v>
       </c>
       <c r="E96" t="n">
-        <v>0.0000314043394856355</v>
+        <v>0.0000313945360272819</v>
       </c>
       <c r="F96" t="n">
-        <v>0.0015198173048337</v>
+        <v>0.00151934286512578</v>
       </c>
       <c r="G96" t="s">
         <v>101</v>
@@ -2964,19 +2964,19 @@
         <v>564.26868346526</v>
       </c>
       <c r="B97" t="n">
-        <v>-1.42594970741328</v>
+        <v>-1.4259498052092</v>
       </c>
       <c r="C97" t="n">
-        <v>0.24132570463776</v>
+        <v>0.241316161958447</v>
       </c>
       <c r="D97" t="n">
-        <v>-5.90881816569722</v>
+        <v>-5.90905223105088</v>
       </c>
       <c r="E97" t="n">
-        <v>0.00000000344570783126206</v>
+        <v>0.00000000344081602282339</v>
       </c>
       <c r="F97" t="n">
-        <v>0.000000489844286512094</v>
+        <v>0.000000489148863530304</v>
       </c>
       <c r="G97" t="s">
         <v>102</v>
@@ -2987,19 +2987,19 @@
         <v>210.91191140456</v>
       </c>
       <c r="B98" t="n">
-        <v>1.74369424416247</v>
+        <v>1.74369420477874</v>
       </c>
       <c r="C98" t="n">
-        <v>0.249385539200209</v>
+        <v>0.249378267613802</v>
       </c>
       <c r="D98" t="n">
-        <v>6.99196212320321</v>
+        <v>6.99216584293181</v>
       </c>
       <c r="E98" t="n">
-        <v>0.00000000000271068073357854</v>
+        <v>0.00000000000270674640450432</v>
       </c>
       <c r="F98" t="n">
-        <v>0.000000000634697921177022</v>
+        <v>0.000000000633776709595849</v>
       </c>
       <c r="G98" t="s">
         <v>103</v>
@@ -3010,19 +3010,19 @@
         <v>70.5428880285636</v>
       </c>
       <c r="B99" t="n">
-        <v>1.76305719435121</v>
+        <v>1.76305747954438</v>
       </c>
       <c r="C99" t="n">
-        <v>0.30540916623849</v>
+        <v>0.305404623868937</v>
       </c>
       <c r="D99" t="n">
-        <v>5.77277105355268</v>
+        <v>5.77285784743386</v>
       </c>
       <c r="E99" t="n">
-        <v>0.00000000779783622609357</v>
+        <v>0.00000000779381911905492</v>
       </c>
       <c r="F99" t="n">
-        <v>0.00000100940771050294</v>
+        <v>0.00000100888770742758</v>
       </c>
       <c r="G99" t="s">
         <v>104</v>
@@ -3033,19 +3033,19 @@
         <v>170.042381642369</v>
       </c>
       <c r="B100" t="n">
-        <v>1.13041463369276</v>
+        <v>1.13041463047551</v>
       </c>
       <c r="C100" t="n">
-        <v>0.347181821636651</v>
+        <v>0.347166979640577</v>
       </c>
       <c r="D100" t="n">
-        <v>3.25597298949544</v>
+        <v>3.25611217877297</v>
       </c>
       <c r="E100" t="n">
-        <v>0.00113004501239141</v>
+        <v>0.00112949116344206</v>
       </c>
       <c r="F100" t="n">
-        <v>0.0285510967560928</v>
+        <v>0.0285456481021023</v>
       </c>
       <c r="G100" t="s">
         <v>105</v>
@@ -3056,19 +3056,19 @@
         <v>109.353891821556</v>
       </c>
       <c r="B101" t="n">
-        <v>2.65000071929163</v>
+        <v>2.6500005388869</v>
       </c>
       <c r="C101" t="n">
-        <v>0.318390808937305</v>
+        <v>0.318380486957805</v>
       </c>
       <c r="D101" t="n">
-        <v>8.32310683884549</v>
+        <v>8.32337610953557</v>
       </c>
       <c r="E101" t="n">
-        <v>0.0000000000000000856871461907848</v>
+        <v>0.0000000000000000854926275328463</v>
       </c>
       <c r="F101" t="n">
-        <v>0.0000000000000378975206013799</v>
+        <v>0.0000000000000378522649632544</v>
       </c>
       <c r="G101" t="s">
         <v>106</v>
@@ -3079,19 +3079,19 @@
         <v>124.805075192301</v>
       </c>
       <c r="B102" t="n">
-        <v>1.69182513508703</v>
+        <v>1.69182553625926</v>
       </c>
       <c r="C102" t="n">
-        <v>0.290906117147622</v>
+        <v>0.290897598053977</v>
       </c>
       <c r="D102" t="n">
-        <v>5.81570835180652</v>
+        <v>5.81588004705814</v>
       </c>
       <c r="E102" t="n">
-        <v>0.00000000603776565189474</v>
+        <v>0.00000000603157085782607</v>
       </c>
       <c r="F102" t="n">
-        <v>0.000000808725394372941</v>
+        <v>0.00000080792674797557</v>
       </c>
       <c r="G102" t="s">
         <v>107</v>
@@ -3102,19 +3102,19 @@
         <v>64.9223952689821</v>
       </c>
       <c r="B103" t="n">
-        <v>-1.55008688828091</v>
+        <v>-1.55008569757543</v>
       </c>
       <c r="C103" t="n">
-        <v>0.473090936367179</v>
+        <v>0.473069787994197</v>
       </c>
       <c r="D103" t="n">
-        <v>-3.2765093750979</v>
+        <v>-3.27665333300558</v>
       </c>
       <c r="E103" t="n">
-        <v>0.00105098823427573</v>
+        <v>0.001050452578257</v>
       </c>
       <c r="F103" t="n">
-        <v>0.0270336585882683</v>
+        <v>0.0270198803731955</v>
       </c>
       <c r="G103" t="s">
         <v>108</v>
@@ -3125,19 +3125,19 @@
         <v>197.351939227944</v>
       </c>
       <c r="B104" t="n">
-        <v>1.40015525659189</v>
+        <v>1.40015525988916</v>
       </c>
       <c r="C104" t="n">
-        <v>0.178720935396321</v>
+        <v>0.178720786890416</v>
       </c>
       <c r="D104" t="n">
-        <v>7.83431025294821</v>
+        <v>7.83431678122406</v>
       </c>
       <c r="E104" t="n">
-        <v>0.00000000000000471423408019055</v>
+        <v>0.00000000000000471398916946135</v>
       </c>
       <c r="F104" t="n">
-        <v>0.00000000000178714369106652</v>
+        <v>0.00000000000178705084657532</v>
       </c>
       <c r="G104" t="s">
         <v>109</v>
@@ -3148,19 +3148,19 @@
         <v>649.618931802309</v>
       </c>
       <c r="B105" t="n">
-        <v>-1.14772664611721</v>
+        <v>-1.14772663433589</v>
       </c>
       <c r="C105" t="n">
-        <v>0.147969605488892</v>
+        <v>0.147967856976225</v>
       </c>
       <c r="D105" t="n">
-        <v>-7.75650271097983</v>
+        <v>-7.75659428871975</v>
       </c>
       <c r="E105" t="n">
-        <v>0.00000000000000873034443526827</v>
+        <v>0.00000000000000872404540499368</v>
       </c>
       <c r="F105" t="n">
-        <v>0.00000000000302183791518134</v>
+        <v>0.00000000000301965762909368</v>
       </c>
       <c r="G105" t="s">
         <v>110</v>
@@ -3171,19 +3171,19 @@
         <v>59.2713822112522</v>
       </c>
       <c r="B106" t="n">
-        <v>1.33970592599714</v>
+        <v>1.33970580052891</v>
       </c>
       <c r="C106" t="n">
-        <v>0.274268935190021</v>
+        <v>0.274270045109596</v>
       </c>
       <c r="D106" t="n">
-        <v>4.88464333399244</v>
+        <v>4.88462310929207</v>
       </c>
       <c r="E106" t="n">
-        <v>0.00000103616243941587</v>
+        <v>0.00000103626879659018</v>
       </c>
       <c r="F106" t="n">
-        <v>0.0000774584218242587</v>
+        <v>0.0000774623088230461</v>
       </c>
       <c r="G106" t="s">
         <v>111</v>
@@ -3194,19 +3194,19 @@
         <v>77.1989769826335</v>
       </c>
       <c r="B107" t="n">
-        <v>-1.38011182834851</v>
+        <v>-1.38011247600989</v>
       </c>
       <c r="C107" t="n">
-        <v>0.386649158132938</v>
+        <v>0.386635574039859</v>
       </c>
       <c r="D107" t="n">
-        <v>-3.56941635412536</v>
+        <v>-3.56954343747896</v>
       </c>
       <c r="E107" t="n">
-        <v>0.00035777742770429</v>
+        <v>0.000357603921428622</v>
       </c>
       <c r="F107" t="n">
-        <v>0.0113026432617216</v>
+        <v>0.0112971619781479</v>
       </c>
       <c r="G107" t="s">
         <v>112</v>
@@ -3217,19 +3217,19 @@
         <v>130.476147348993</v>
       </c>
       <c r="B108" t="n">
-        <v>1.0541331985676</v>
+        <v>1.05413304053008</v>
       </c>
       <c r="C108" t="n">
-        <v>0.174726183956894</v>
+        <v>0.174729867780678</v>
       </c>
       <c r="D108" t="n">
-        <v>6.03305798075271</v>
+        <v>6.03292988153135</v>
       </c>
       <c r="E108" t="n">
-        <v>0.00000000160885656492869</v>
+        <v>0.00000000161013293028509</v>
       </c>
       <c r="F108" t="n">
-        <v>0.000000243963945017091</v>
+        <v>0.000000244157490628563</v>
       </c>
       <c r="G108" t="s">
         <v>113</v>
@@ -3240,19 +3240,19 @@
         <v>2452.19412553395</v>
       </c>
       <c r="B109" t="n">
-        <v>1.98788125723288</v>
+        <v>1.98788126279647</v>
       </c>
       <c r="C109" t="n">
-        <v>0.200903643251388</v>
+        <v>0.200896164773985</v>
       </c>
       <c r="D109" t="n">
-        <v>9.89469989225366</v>
+        <v>9.89506825594657</v>
       </c>
       <c r="E109" t="n">
-        <v>0.0000000000000000000000438924896576528</v>
+        <v>0.0000000000000000000000437312000629178</v>
       </c>
       <c r="F109" t="n">
-        <v>0.0000000000000000000279542488131659</v>
+        <v>0.0000000000000000000278515266960711</v>
       </c>
       <c r="G109" t="s">
         <v>114</v>
@@ -3263,19 +3263,19 @@
         <v>183.549457846273</v>
       </c>
       <c r="B110" t="n">
-        <v>1.04962425353881</v>
+        <v>1.04962433409311</v>
       </c>
       <c r="C110" t="n">
-        <v>0.196973599286118</v>
+        <v>0.19697159930649</v>
       </c>
       <c r="D110" t="n">
-        <v>5.32875602285239</v>
+        <v>5.32881053811158</v>
       </c>
       <c r="E110" t="n">
-        <v>0.0000000988877276419482</v>
+        <v>0.0000000988580547401743</v>
       </c>
       <c r="F110" t="n">
-        <v>0.00000997155451194794</v>
+        <v>0.00000997260823421916</v>
       </c>
       <c r="G110" t="s">
         <v>115</v>
@@ -3286,19 +3286,19 @@
         <v>133.243916439747</v>
       </c>
       <c r="B111" t="n">
-        <v>-1.58604556378518</v>
+        <v>-1.58604557662438</v>
       </c>
       <c r="C111" t="n">
-        <v>0.210118127097738</v>
+        <v>0.210117690884003</v>
       </c>
       <c r="D111" t="n">
-        <v>-7.54835189944093</v>
+        <v>-7.5483676312623</v>
       </c>
       <c r="E111" t="n">
-        <v>0.0000000000000440800576883425</v>
+        <v>0.0000000000000440747346317267</v>
       </c>
       <c r="F111" t="n">
-        <v>0.0000000000134969745868037</v>
+        <v>0.0000000000134953447078145</v>
       </c>
       <c r="G111" t="s">
         <v>116</v>
@@ -3309,19 +3309,19 @@
         <v>301.311242022388</v>
       </c>
       <c r="B112" t="n">
-        <v>1.40680805616102</v>
+        <v>1.40680813109611</v>
       </c>
       <c r="C112" t="n">
-        <v>0.281718074032909</v>
+        <v>0.281706285032593</v>
       </c>
       <c r="D112" t="n">
-        <v>4.99367341264972</v>
+        <v>4.99388265665904</v>
       </c>
       <c r="E112" t="n">
-        <v>0.00000059241543427494</v>
+        <v>0.000000591773612408258</v>
       </c>
       <c r="F112" t="n">
-        <v>0.000047600271855231</v>
+        <v>0.000047586966953355</v>
       </c>
       <c r="G112" t="s">
         <v>117</v>
@@ -3332,19 +3332,19 @@
         <v>429.403863079329</v>
       </c>
       <c r="B113" t="n">
-        <v>1.36612205396656</v>
+        <v>1.36612207939136</v>
       </c>
       <c r="C113" t="n">
-        <v>0.225817106548744</v>
+        <v>0.225809581805974</v>
       </c>
       <c r="D113" t="n">
-        <v>6.04968363489182</v>
+        <v>6.04988534350681</v>
       </c>
       <c r="E113" t="n">
-        <v>0.00000000145130550470532</v>
+        <v>0.00000000144948957560321</v>
       </c>
       <c r="F113" t="n">
-        <v>0.000000226545943587433</v>
+        <v>0.000000226262480615238</v>
       </c>
       <c r="G113" t="s">
         <v>118</v>
@@ -3355,19 +3355,19 @@
         <v>131.325084510812</v>
       </c>
       <c r="B114" t="n">
-        <v>-3.69902438963636</v>
+        <v>-3.69902462747369</v>
       </c>
       <c r="C114" t="n">
-        <v>0.306296860400249</v>
+        <v>0.306289612678429</v>
       </c>
       <c r="D114" t="n">
-        <v>-12.0765991032449</v>
+        <v>-12.0768856479546</v>
       </c>
       <c r="E114" t="n">
-        <v>0.0000000000000000000000000000000014040785562043</v>
+        <v>0.00000000000000000000000000000000139919534367581</v>
       </c>
       <c r="F114" t="n">
-        <v>0.00000000000000000000000000000171967221322191</v>
+        <v>0.00000000000000000000000000000171369140476972</v>
       </c>
       <c r="G114" t="s">
         <v>119</v>
@@ -3378,19 +3378,19 @@
         <v>130.695122095063</v>
       </c>
       <c r="B115" t="n">
-        <v>1.38344589675669</v>
+        <v>1.38344588157631</v>
       </c>
       <c r="C115" t="n">
-        <v>0.264188987149617</v>
+        <v>0.264182263919924</v>
       </c>
       <c r="D115" t="n">
-        <v>5.23657670852573</v>
+        <v>5.23670991779995</v>
       </c>
       <c r="E115" t="n">
-        <v>0.000000163582272270488</v>
+        <v>0.000000163464303018729</v>
       </c>
       <c r="F115" t="n">
-        <v>0.0000157851935702468</v>
+        <v>0.0000157738098949345</v>
       </c>
       <c r="G115" t="s">
         <v>120</v>
@@ -3401,19 +3401,19 @@
         <v>51.5269157092482</v>
       </c>
       <c r="B116" t="n">
-        <v>-1.38702461730082</v>
+        <v>-1.38702531317921</v>
       </c>
       <c r="C116" t="n">
-        <v>0.419800586979617</v>
+        <v>0.41978745697189</v>
       </c>
       <c r="D116" t="n">
-        <v>-3.3040082846958</v>
+        <v>-3.30411328433782</v>
       </c>
       <c r="E116" t="n">
-        <v>0.000953130155380386</v>
+        <v>0.000952773235248046</v>
       </c>
       <c r="F116" t="n">
-        <v>0.0249600959440239</v>
+        <v>0.0249507490980582</v>
       </c>
       <c r="G116" t="s">
         <v>121</v>
@@ -3424,19 +3424,19 @@
         <v>94.0494890122973</v>
       </c>
       <c r="B117" t="n">
-        <v>-1.38420553138372</v>
+        <v>-1.38420540166371</v>
       </c>
       <c r="C117" t="n">
-        <v>0.382892161374512</v>
+        <v>0.382896345359229</v>
       </c>
       <c r="D117" t="n">
-        <v>-3.61513154621572</v>
+        <v>-3.6150917041662</v>
       </c>
       <c r="E117" t="n">
-        <v>0.000300195151060191</v>
+        <v>0.000300241322931702</v>
       </c>
       <c r="F117" t="n">
-        <v>0.00983620252322056</v>
+        <v>0.00983702518295657</v>
       </c>
       <c r="G117" t="s">
         <v>122</v>
@@ -3447,19 +3447,19 @@
         <v>594.932914831975</v>
       </c>
       <c r="B118" t="n">
-        <v>1.29634274046304</v>
+        <v>1.29634285977207</v>
       </c>
       <c r="C118" t="n">
-        <v>0.210742507268904</v>
+        <v>0.21073529651267</v>
       </c>
       <c r="D118" t="n">
-        <v>6.1513111771463</v>
+        <v>6.15152222349296</v>
       </c>
       <c r="E118" t="n">
-        <v>0.000000000768449773913646</v>
+        <v>0.000000000767427700497457</v>
       </c>
       <c r="F118" t="n">
-        <v>0.000000128792182107927</v>
+        <v>0.000000128620882603374</v>
       </c>
       <c r="G118" t="s">
         <v>123</v>
@@ -3470,19 +3470,19 @@
         <v>51.7567763020407</v>
       </c>
       <c r="B119" t="n">
-        <v>4.63912648168132</v>
+        <v>4.63912672423082</v>
       </c>
       <c r="C119" t="n">
-        <v>0.587542523772894</v>
+        <v>0.587517109039832</v>
       </c>
       <c r="D119" t="n">
-        <v>7.89581399468969</v>
+        <v>7.89615596354709</v>
       </c>
       <c r="E119" t="n">
-        <v>0.00000000000000288426565119276</v>
+        <v>0.00000000000000287636725014756</v>
       </c>
       <c r="F119" t="n">
-        <v>0.00000000000112007994386076</v>
+        <v>0.00000000000111701266724023</v>
       </c>
       <c r="G119" t="s">
         <v>124</v>
@@ -3493,19 +3493,19 @@
         <v>54.2877595806348</v>
       </c>
       <c r="B120" t="n">
-        <v>1.5090560161768</v>
+        <v>1.50905570021341</v>
       </c>
       <c r="C120" t="n">
-        <v>0.326810945174628</v>
+        <v>0.326807350195818</v>
       </c>
       <c r="D120" t="n">
-        <v>4.61751981828654</v>
+        <v>4.61756964557009</v>
       </c>
       <c r="E120" t="n">
-        <v>0.00000388353603119316</v>
+        <v>0.00000388260394785591</v>
       </c>
       <c r="F120" t="n">
-        <v>0.000244401820903785</v>
+        <v>0.000244343162283644</v>
       </c>
       <c r="G120" t="s">
         <v>125</v>
@@ -3516,19 +3516,19 @@
         <v>277.390046865757</v>
       </c>
       <c r="B121" t="n">
-        <v>1.05092518524386</v>
+        <v>1.05092510643977</v>
       </c>
       <c r="C121" t="n">
-        <v>0.142963151186818</v>
+        <v>0.142964848753485</v>
       </c>
       <c r="D121" t="n">
-        <v>7.35102141019925</v>
+        <v>7.35093357285248</v>
       </c>
       <c r="E121" t="n">
-        <v>0.000000000000196697907357531</v>
+        <v>0.000000000000196827226265964</v>
       </c>
       <c r="F121" t="n">
-        <v>0.0000000000539969669128726</v>
+        <v>0.0000000000540324671828739</v>
       </c>
       <c r="G121" t="s">
         <v>126</v>
@@ -3539,19 +3539,19 @@
         <v>441.933484289599</v>
       </c>
       <c r="B122" t="n">
-        <v>-1.21299814647277</v>
+        <v>-1.2129982191085</v>
       </c>
       <c r="C122" t="n">
-        <v>0.162811479494848</v>
+        <v>0.162809299517721</v>
       </c>
       <c r="D122" t="n">
-        <v>-7.45032322190254</v>
+        <v>-7.45042342606767</v>
       </c>
       <c r="E122" t="n">
-        <v>0.0000000000000931118279828568</v>
+        <v>0.0000000000000930411306244629</v>
       </c>
       <c r="F122" t="n">
-        <v>0.0000000000274541949100564</v>
+        <v>0.0000000000274333496630129</v>
       </c>
       <c r="G122" t="s">
         <v>127</v>
@@ -3562,19 +3562,19 @@
         <v>414.055116388387</v>
       </c>
       <c r="B123" t="n">
-        <v>1.0800683534502</v>
+        <v>1.08006846324163</v>
       </c>
       <c r="C123" t="n">
-        <v>0.17658603412037</v>
+        <v>0.176582629653977</v>
       </c>
       <c r="D123" t="n">
-        <v>6.11638603715383</v>
+        <v>6.11650458121551</v>
       </c>
       <c r="E123" t="n">
-        <v>0.000000000957212836166942</v>
+        <v>0.000000000956501384406473</v>
       </c>
       <c r="F123" t="n">
-        <v>0.000000155517783443368</v>
+        <v>0.000000155402194311427</v>
       </c>
       <c r="G123" t="s">
         <v>128</v>
@@ -3585,19 +3585,19 @@
         <v>53.2777711830204</v>
       </c>
       <c r="B124" t="n">
-        <v>-1.20348942193984</v>
+        <v>-1.20348932787561</v>
       </c>
       <c r="C124" t="n">
-        <v>0.315775593728882</v>
+        <v>0.31577353943751</v>
       </c>
       <c r="D124" t="n">
-        <v>-3.81121735131033</v>
+        <v>-3.81124184762092</v>
       </c>
       <c r="E124" t="n">
-        <v>0.000138284110385062</v>
+        <v>0.000138270405519576</v>
       </c>
       <c r="F124" t="n">
-        <v>0.00530544483265292</v>
+        <v>0.00530491902815106</v>
       </c>
       <c r="G124" t="s">
         <v>129</v>
@@ -3608,19 +3608,19 @@
         <v>50.6118390602331</v>
       </c>
       <c r="B125" t="n">
-        <v>2.84511169552803</v>
+        <v>2.84511275504429</v>
       </c>
       <c r="C125" t="n">
-        <v>0.475119426669117</v>
+        <v>0.475102835785722</v>
       </c>
       <c r="D125" t="n">
-        <v>5.98820325128366</v>
+        <v>5.98841459310395</v>
       </c>
       <c r="E125" t="n">
-        <v>0.00000000212171819263364</v>
+        <v>0.00000000211896358718239</v>
       </c>
       <c r="F125" t="n">
-        <v>0.000000312796269102897</v>
+        <v>0.000000312390168843686</v>
       </c>
       <c r="G125" t="s">
         <v>130</v>
@@ -3634,16 +3634,16 @@
         <v>2.81743455169951</v>
       </c>
       <c r="C126" t="n">
-        <v>0.837888875192162</v>
+        <v>0.837888875192161</v>
       </c>
       <c r="D126" t="n">
         <v>3.36253963397397</v>
       </c>
       <c r="E126" t="n">
-        <v>0.000772290388563105</v>
+        <v>0.000772290388563106</v>
       </c>
       <c r="F126" t="n">
-        <v>0.0213040614296989</v>
+        <v>0.0213076796806893</v>
       </c>
       <c r="G126" t="s">
         <v>131</v>
@@ -3654,19 +3654,19 @@
         <v>53.2002490179201</v>
       </c>
       <c r="B127" t="n">
-        <v>1.61288524246302</v>
+        <v>1.61288541924191</v>
       </c>
       <c r="C127" t="n">
-        <v>0.351516422754727</v>
+        <v>0.35151037609903</v>
       </c>
       <c r="D127" t="n">
-        <v>4.58836383752239</v>
+        <v>4.58844326913273</v>
       </c>
       <c r="E127" t="n">
-        <v>0.00000446733542434912</v>
+        <v>0.00000446563625969279</v>
       </c>
       <c r="F127" t="n">
-        <v>0.000278936920103869</v>
+        <v>0.000278830825595406</v>
       </c>
       <c r="G127" t="s">
         <v>132</v>
@@ -3677,19 +3677,19 @@
         <v>58.630012570833</v>
       </c>
       <c r="B128" t="n">
-        <v>1.38557408293711</v>
+        <v>1.38557442224573</v>
       </c>
       <c r="C128" t="n">
-        <v>0.342556575863087</v>
+        <v>0.342550241996009</v>
       </c>
       <c r="D128" t="n">
-        <v>4.04480363410363</v>
+        <v>4.04487941439516</v>
       </c>
       <c r="E128" t="n">
-        <v>0.0000523669984040464</v>
+        <v>0.0000523500625874511</v>
       </c>
       <c r="F128" t="n">
-        <v>0.00236200382036608</v>
+        <v>0.00236123993347704</v>
       </c>
       <c r="G128" t="s">
         <v>133</v>
@@ -3700,19 +3700,19 @@
         <v>62.2364239753687</v>
       </c>
       <c r="B129" t="n">
-        <v>-1.8105061146028</v>
+        <v>-1.81050645130356</v>
       </c>
       <c r="C129" t="n">
-        <v>0.346181522739072</v>
+        <v>0.34617389150211</v>
       </c>
       <c r="D129" t="n">
-        <v>-5.22993284066012</v>
+        <v>-5.23004910464925</v>
       </c>
       <c r="E129" t="n">
-        <v>0.00000016957163053372</v>
+        <v>0.000000169465020268151</v>
       </c>
       <c r="F129" t="n">
-        <v>0.0000162645753093849</v>
+        <v>0.0000162543497151175</v>
       </c>
       <c r="G129" t="s">
         <v>134</v>
@@ -3723,19 +3723,19 @@
         <v>66.4670390550662</v>
       </c>
       <c r="B130" t="n">
-        <v>1.0406964200488</v>
+        <v>1.0406962155494</v>
       </c>
       <c r="C130" t="n">
-        <v>0.33478359392842</v>
+        <v>0.334776373181055</v>
       </c>
       <c r="D130" t="n">
-        <v>3.10856457401944</v>
+        <v>3.10863101138433</v>
       </c>
       <c r="E130" t="n">
-        <v>0.00187998558418258</v>
+        <v>0.00187956293882378</v>
       </c>
       <c r="F130" t="n">
-        <v>0.0422188017931666</v>
+        <v>0.0422338420843711</v>
       </c>
       <c r="G130" t="s">
         <v>135</v>

</xml_diff>